<commit_message>
warenkorbrabatt bei 5/10 Artikeln. Datenschutzprüfung. Entfernung Zahlungsarten
</commit_message>
<xml_diff>
--- a/Webshop_Checkliste.xlsx
+++ b/Webshop_Checkliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Webprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0FAF8-B862-DD4F-A746-C5560184AED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124889C1-1391-5E4B-84F1-89DE3509A4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="680" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Webshop Checkliste (detailliert" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
   <si>
     <t>Nr</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Florian/(Kimi)/Andy</t>
+  </si>
+  <si>
+    <t>Punkte als Rabatt einlösen</t>
   </si>
 </sst>
 </file>
@@ -709,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1430,6 +1433,9 @@
       <c r="D42" t="s">
         <v>71</v>
       </c>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
       <c r="F42" t="s">
         <v>108</v>
       </c>
@@ -1447,6 +1453,9 @@
       <c r="D43" t="s">
         <v>72</v>
       </c>
+      <c r="E43" t="s">
+        <v>105</v>
+      </c>
       <c r="F43" t="s">
         <v>108</v>
       </c>
@@ -1493,10 +1502,13 @@
         <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>78</v>
+        <v>110</v>
+      </c>
+      <c r="E46" t="s">
+        <v>105</v>
       </c>
       <c r="F46" t="s">
         <v>108</v>
@@ -1510,10 +1522,13 @@
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="E47" t="s">
+        <v>105</v>
       </c>
       <c r="F47" t="s">
         <v>108</v>
@@ -1527,10 +1542,13 @@
         <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="E48" t="s">
+        <v>105</v>
       </c>
       <c r="F48" t="s">
         <v>108</v>
@@ -1544,10 +1562,13 @@
         <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E49" t="s">
+        <v>105</v>
       </c>
       <c r="F49" t="s">
         <v>108</v>
@@ -1561,10 +1582,10 @@
         <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F50" t="s">
         <v>108</v>
@@ -1572,16 +1593,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F51" t="s">
         <v>108</v>
@@ -1595,10 +1616,10 @@
         <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F52" t="s">
         <v>108</v>
@@ -1612,27 +1633,27 @@
         <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
         <v>106</v>
@@ -1646,10 +1667,10 @@
         <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F55" t="s">
         <v>106</v>
@@ -1663,10 +1684,10 @@
         <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F56" t="s">
         <v>106</v>
@@ -1674,19 +1695,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>98</v>
-      </c>
-      <c r="E57" t="s">
-        <v>105</v>
+        <v>96</v>
+      </c>
+      <c r="F57" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1697,10 +1718,10 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D58" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E58" t="s">
         <v>105</v>
@@ -1708,16 +1729,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E59" t="s">
         <v>105</v>
@@ -1731,18 +1752,35 @@
         <v>101</v>
       </c>
       <c r="C60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" t="s">
         <v>103</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>104</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E2:E60 F53" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F54 E2:E61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Ja,Nein"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
GutscheidCode Tabelle. Gutscheinlogik implementiert. Anpassung ArtikelTabelle.
</commit_message>
<xml_diff>
--- a/Webshop_Checkliste.xlsx
+++ b/Webshop_Checkliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Webprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124889C1-1391-5E4B-84F1-89DE3509A4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528131CB-3973-A241-82CF-F7D31E84E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,9 +1507,6 @@
       <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="E46" t="s">
-        <v>105</v>
-      </c>
       <c r="F46" t="s">
         <v>108</v>
       </c>
@@ -1604,6 +1601,9 @@
       <c r="D51" t="s">
         <v>85</v>
       </c>
+      <c r="E51" t="s">
+        <v>105</v>
+      </c>
       <c r="F51" t="s">
         <v>108</v>
       </c>
@@ -1780,7 +1780,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="F54 E2:E61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="F54 E47:E61 E2:E45" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Ja,Nein"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Mail erstellung und Rechnungsversand
</commit_message>
<xml_diff>
--- a/Webshop_Checkliste.xlsx
+++ b/Webshop_Checkliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Webprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528131CB-3973-A241-82CF-F7D31E84E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4DE03-5B07-134F-9607-EB36EDA352E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="111">
   <si>
     <t>Nr</t>
   </si>
@@ -715,7 +715,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,6 +1584,9 @@
       <c r="D50" t="s">
         <v>84</v>
       </c>
+      <c r="E50" t="s">
+        <v>105</v>
+      </c>
       <c r="F50" t="s">
         <v>108</v>
       </c>
@@ -1620,6 +1623,9 @@
       </c>
       <c r="D52" t="s">
         <v>88</v>
+      </c>
+      <c r="E52" t="s">
+        <v>105</v>
       </c>
       <c r="F52" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Punkte in Rabatt umwandeln
</commit_message>
<xml_diff>
--- a/Webshop_Checkliste.xlsx
+++ b/Webshop_Checkliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/Webprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4DE03-5B07-134F-9607-EB36EDA352E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8F1A2-15BB-144F-9747-80DBC370E9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="112">
   <si>
     <t>Nr</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Punkte als Rabatt einlösen</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,6 +1510,9 @@
       <c r="D46" t="s">
         <v>110</v>
       </c>
+      <c r="E46" t="s">
+        <v>111</v>
+      </c>
       <c r="F46" t="s">
         <v>108</v>
       </c>
@@ -1643,6 +1649,9 @@
       </c>
       <c r="D53" t="s">
         <v>90</v>
+      </c>
+      <c r="E53" t="s">
+        <v>105</v>
       </c>
       <c r="F53" t="s">
         <v>108</v>

</xml_diff>